<commit_message>
add message when key cell is empty
</commit_message>
<xml_diff>
--- a/inputs/sample2.xlsx
+++ b/inputs/sample2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zengjf\github\XLBoom\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA8F79C-1834-4D2D-BC98-AC69C1DEA3E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7905D45-9EBF-4253-AFFA-1C54923F8944}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="98">
   <si>
     <t>Item</t>
   </si>
@@ -1283,8 +1283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD194"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1405,6 +1405,9 @@
         <f>"0R,SMD0603"</f>
         <v>0R,SMD0603</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G5" s="3">
         <v>2</v>
       </c>

</xml_diff>